<commit_message>
DBank na mão com alguns tapa-buracos
</commit_message>
<xml_diff>
--- a/DBank.xlsx
+++ b/DBank.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D831C8F9-FDB1-4EDA-AB54-7947E99AF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D2F1F6C-6191-4086-9AEE-63C202AB8468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -77,10 +83,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G362" workbookViewId="0">
-      <selection activeCell="W358" sqref="W358:W392"/>
+    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
+      <selection activeCell="O362" sqref="O362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,6 +730,10 @@
       <c r="B10">
         <v>0.22963</v>
       </c>
+      <c r="C10" s="3">
+        <f>(C11+C9)/2</f>
+        <v>0.23122999999999999</v>
+      </c>
       <c r="D10">
         <v>0.22844</v>
       </c>
@@ -736,6 +748,10 @@
       </c>
       <c r="N10">
         <v>-0.56599999999999995</v>
+      </c>
+      <c r="O10" s="3">
+        <f>(O11+O9)/2</f>
+        <v>-0.56905000000000006</v>
       </c>
       <c r="P10">
         <v>-0.56599999999999995</v>
@@ -1037,6 +1053,10 @@
       <c r="E16">
         <v>0.11975</v>
       </c>
+      <c r="F16" s="3">
+        <f>(F17+F15)/2</f>
+        <v>0.14124999999999999</v>
+      </c>
       <c r="I16">
         <v>1.8519999999999998E-2</v>
       </c>
@@ -1060,6 +1080,10 @@
       </c>
       <c r="Q16">
         <v>-0.2303</v>
+      </c>
+      <c r="R16" s="3">
+        <f>(R17+R15)/2</f>
+        <v>-0.41354999999999997</v>
       </c>
       <c r="U16">
         <v>-1.0274000000000001</v>
@@ -1217,6 +1241,10 @@
       <c r="G19">
         <v>8.8900000000000007E-2</v>
       </c>
+      <c r="H19" s="3">
+        <f>(H20+H18)/2</f>
+        <v>3.1890000000000002E-2</v>
+      </c>
       <c r="I19">
         <v>1.9730000000000001E-2</v>
       </c>
@@ -1246,6 +1274,10 @@
       </c>
       <c r="S19">
         <v>-0.40649999999999997</v>
+      </c>
+      <c r="T19" s="3">
+        <f>(T20+T18)/2</f>
+        <v>-0.62870000000000004</v>
       </c>
       <c r="U19">
         <v>-0.66279999999999994</v>
@@ -1270,6 +1302,14 @@
       <c r="D20">
         <v>9.4280000000000003E-2</v>
       </c>
+      <c r="E20" s="3">
+        <f>(E21+E19)/2</f>
+        <v>9.1265000000000013E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <f>(F21+F19)/2</f>
+        <v>6.9695000000000007E-2</v>
+      </c>
       <c r="G20">
         <v>2.8289999999999999E-2</v>
       </c>
@@ -1296,6 +1336,14 @@
       </c>
       <c r="P20">
         <v>-0.35320000000000001</v>
+      </c>
+      <c r="Q20" s="3">
+        <f>(Q21+Q19)/2</f>
+        <v>-0.40959999999999996</v>
+      </c>
+      <c r="R20" s="3">
+        <f>(R21+R19)/2</f>
+        <v>-0.39439999999999997</v>
       </c>
       <c r="S20">
         <v>-0.53310000000000002</v>
@@ -1781,6 +1829,10 @@
       <c r="A28">
         <v>-1</v>
       </c>
+      <c r="B28" s="3">
+        <f>(B29+B27)/2</f>
+        <v>2.1045000000000001E-2</v>
+      </c>
       <c r="C28">
         <v>1.3050000000000001E-2</v>
       </c>
@@ -1810,6 +1862,10 @@
       </c>
       <c r="M28">
         <v>-1</v>
+      </c>
+      <c r="N28" s="3">
+        <f>(N29+N27)/2</f>
+        <v>0.19980000000000001</v>
       </c>
       <c r="O28">
         <v>0.2944</v>
@@ -2006,6 +2062,10 @@
       <c r="J31">
         <v>5.6499999999999996E-3</v>
       </c>
+      <c r="K31" s="3">
+        <f>(K32+K30)/2</f>
+        <v>5.7250000000000001E-3</v>
+      </c>
       <c r="M31">
         <v>2</v>
       </c>
@@ -2035,6 +2095,10 @@
       </c>
       <c r="V31">
         <v>0.60950000000000004</v>
+      </c>
+      <c r="W31" s="3">
+        <f>(W32+W30)/2</f>
+        <v>0.60929999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -2523,6 +2587,10 @@
       <c r="C39">
         <v>2.3189999999999999E-2</v>
       </c>
+      <c r="D39" s="3">
+        <f>(D40+D38)/2</f>
+        <v>2.2245000000000001E-2</v>
+      </c>
       <c r="E39">
         <v>2.0420000000000001E-2</v>
       </c>
@@ -2541,6 +2609,10 @@
       <c r="J39">
         <v>1.391E-2</v>
       </c>
+      <c r="K39" s="3">
+        <f>(K40+K38)/2</f>
+        <v>1.3105E-2</v>
+      </c>
       <c r="M39">
         <v>10</v>
       </c>
@@ -2550,6 +2622,10 @@
       <c r="O39">
         <v>1.3123</v>
       </c>
+      <c r="P39" s="3">
+        <f>(P40+P38)/2</f>
+        <v>1.3077999999999999</v>
+      </c>
       <c r="Q39">
         <v>1.3197000000000001</v>
       </c>
@@ -2567,6 +2643,10 @@
       </c>
       <c r="V39">
         <v>1.4071</v>
+      </c>
+      <c r="W39" s="3">
+        <f>(W40+W38)/2</f>
+        <v>1.4169499999999999</v>
       </c>
     </row>
     <row r="40" spans="1:23">
@@ -3247,6 +3327,10 @@
       <c r="C50">
         <v>0.26384000000000002</v>
       </c>
+      <c r="D50" s="3">
+        <f>(D51+D49)/2</f>
+        <v>0.20052999999999999</v>
+      </c>
       <c r="E50">
         <v>0.19885</v>
       </c>
@@ -3276,6 +3360,10 @@
       </c>
       <c r="O50">
         <v>1.0311999999999999</v>
+      </c>
+      <c r="P50" s="3">
+        <f>(P51+P49)/2</f>
+        <v>0.92409999999999992</v>
       </c>
       <c r="Q50">
         <v>0.70230000000000004</v>
@@ -3634,6 +3722,10 @@
       <c r="B56">
         <v>0.29346</v>
       </c>
+      <c r="C56" s="3">
+        <f>(C57+C55)/2</f>
+        <v>0.3458</v>
+      </c>
       <c r="D56">
         <v>0.29053000000000001</v>
       </c>
@@ -3663,6 +3755,10 @@
       </c>
       <c r="N56">
         <v>0.74080000000000001</v>
+      </c>
+      <c r="O56" s="3">
+        <f>(O57+O55)/2</f>
+        <v>1.2004000000000001</v>
       </c>
       <c r="P56">
         <v>0.73970000000000002</v>
@@ -3714,6 +3810,10 @@
       <c r="H57">
         <v>0.29901</v>
       </c>
+      <c r="I57" s="3">
+        <f>(I58+I56)/2</f>
+        <v>0.31834000000000001</v>
+      </c>
       <c r="J57">
         <v>0.28397</v>
       </c>
@@ -3743,6 +3843,10 @@
       </c>
       <c r="T57">
         <v>0.75449999999999995</v>
+      </c>
+      <c r="U57" s="3">
+        <f>(U58+U56)/2</f>
+        <v>1.2765499999999999</v>
       </c>
       <c r="V57">
         <v>1.3224</v>
@@ -4215,6 +4319,10 @@
       <c r="F70">
         <v>0.21443999999999999</v>
       </c>
+      <c r="G70" s="3">
+        <f>(G71+G69)/2</f>
+        <v>0.18474499999999999</v>
+      </c>
       <c r="K70">
         <v>3.746E-2</v>
       </c>
@@ -4232,6 +4340,10 @@
       </c>
       <c r="R70">
         <v>-0.53639999999999999</v>
+      </c>
+      <c r="S70" s="3">
+        <f>(S71+S69)/2</f>
+        <v>-0.41925000000000001</v>
       </c>
       <c r="W70">
         <v>-1.3767</v>
@@ -4418,6 +4530,10 @@
       <c r="F74">
         <v>0.15570999999999999</v>
       </c>
+      <c r="G74" s="3">
+        <f>(G75+G73)/2</f>
+        <v>0.143565</v>
+      </c>
       <c r="I74">
         <v>1.9720000000000001E-2</v>
       </c>
@@ -4444,6 +4560,10 @@
       </c>
       <c r="R74">
         <v>-0.43059999999999998</v>
+      </c>
+      <c r="S74" s="3">
+        <f>(S75+S73)/2</f>
+        <v>-0.34455000000000002</v>
       </c>
       <c r="U74">
         <v>-1.1658999999999999</v>
@@ -4471,6 +4591,10 @@
       <c r="E75">
         <v>0.14671000000000001</v>
       </c>
+      <c r="F75" s="3">
+        <f>(F76+F74)/2</f>
+        <v>0.14178499999999999</v>
+      </c>
       <c r="G75">
         <v>0.11554</v>
       </c>
@@ -4497,6 +4621,10 @@
       </c>
       <c r="Q75">
         <v>-0.41470000000000001</v>
+      </c>
+      <c r="R75" s="3">
+        <f>(R76+R74)/2</f>
+        <v>-0.41154999999999997</v>
       </c>
       <c r="S75">
         <v>-0.23930000000000001</v>
@@ -4654,6 +4782,10 @@
       <c r="F78">
         <v>9.486E-2</v>
       </c>
+      <c r="H78" s="3">
+        <f>(H79+H77)/2</f>
+        <v>3.6600000000000001E-2</v>
+      </c>
       <c r="I78">
         <v>1.9910000000000001E-2</v>
       </c>
@@ -4680,6 +4812,10 @@
       </c>
       <c r="R78">
         <v>-0.38390000000000002</v>
+      </c>
+      <c r="T78" s="3">
+        <f>(T79+T77)/2</f>
+        <v>-0.59634999999999994</v>
       </c>
       <c r="U78">
         <v>-0.66779999999999995</v>
@@ -4707,6 +4843,10 @@
       <c r="E79">
         <v>9.393E-2</v>
       </c>
+      <c r="F79" s="3">
+        <f>(F80+F78)/2</f>
+        <v>7.1415000000000006E-2</v>
+      </c>
       <c r="G79">
         <v>1.0789999999999999E-2</v>
       </c>
@@ -4736,6 +4876,10 @@
       </c>
       <c r="Q79">
         <v>-0.38</v>
+      </c>
+      <c r="R79" s="3">
+        <f>(R80+R78)/2</f>
+        <v>-0.38845000000000002</v>
       </c>
       <c r="S79">
         <v>-0.46600000000000003</v>
@@ -5192,6 +5336,10 @@
       <c r="J86">
         <v>6.4900000000000001E-3</v>
       </c>
+      <c r="K86" s="3">
+        <f>(K87+K85)/2</f>
+        <v>6.2500000000000003E-3</v>
+      </c>
       <c r="M86">
         <v>-2</v>
       </c>
@@ -5221,12 +5369,20 @@
       </c>
       <c r="V86">
         <v>0.17380000000000001</v>
+      </c>
+      <c r="W86" s="3">
+        <f>(W87+W85)/2</f>
+        <v>0.17285</v>
       </c>
     </row>
     <row r="87" spans="1:23">
       <c r="A87">
         <v>-1</v>
       </c>
+      <c r="B87" s="3">
+        <f>(B88+B86)/2</f>
+        <v>2.1174999999999999E-2</v>
+      </c>
       <c r="C87">
         <v>1.315E-2</v>
       </c>
@@ -5256,6 +5412,10 @@
       </c>
       <c r="M87">
         <v>-1</v>
+      </c>
+      <c r="N87" s="3">
+        <f>(N88+N86)/2</f>
+        <v>0.19970000000000002</v>
       </c>
       <c r="O87">
         <v>0.2873</v>
@@ -5514,6 +5674,10 @@
       <c r="H91">
         <v>6.5199999999999998E-3</v>
       </c>
+      <c r="I91" s="3">
+        <f>(I92+I90)/2</f>
+        <v>5.9699999999999996E-3</v>
+      </c>
       <c r="J91">
         <v>5.6800000000000002E-3</v>
       </c>
@@ -5543,6 +5707,10 @@
       </c>
       <c r="T91">
         <v>0.746</v>
+      </c>
+      <c r="U91" s="3">
+        <f>(U92+U90)/2</f>
+        <v>0.72570000000000001</v>
       </c>
       <c r="V91">
         <v>0.71230000000000004</v>
@@ -5626,6 +5794,10 @@
       <c r="B93">
         <v>1.8149999999999999E-2</v>
       </c>
+      <c r="C93" s="3">
+        <f>(C94+C92)/2</f>
+        <v>1.4605E-2</v>
+      </c>
       <c r="D93">
         <v>1.277E-2</v>
       </c>
@@ -5655,6 +5827,10 @@
       </c>
       <c r="N93">
         <v>0.92459999999999998</v>
+      </c>
+      <c r="O93" s="3">
+        <f>(O94+O92)/2</f>
+        <v>0.92679999999999996</v>
       </c>
       <c r="P93">
         <v>0.92620000000000002</v>
@@ -5972,6 +6148,10 @@
       <c r="F98">
         <v>1.8360000000000001E-2</v>
       </c>
+      <c r="G98" s="3">
+        <f>(G99+G97)/2</f>
+        <v>1.8024999999999999E-2</v>
+      </c>
       <c r="H98">
         <v>1.7350000000000001E-2</v>
       </c>
@@ -6001,6 +6181,10 @@
       </c>
       <c r="R98">
         <v>1.3460000000000001</v>
+      </c>
+      <c r="S98" s="3">
+        <f>(S99+S97)/2</f>
+        <v>1.3483000000000001</v>
       </c>
       <c r="T98">
         <v>1.3579000000000001</v>
@@ -6028,6 +6212,10 @@
       <c r="D99">
         <v>2.6329999999999999E-2</v>
       </c>
+      <c r="E99" s="3">
+        <f>(E100+E98)/2</f>
+        <v>2.5605000000000003E-2</v>
+      </c>
       <c r="F99">
         <v>2.282E-2</v>
       </c>
@@ -6057,6 +6245,10 @@
       </c>
       <c r="P99">
         <v>1.3504</v>
+      </c>
+      <c r="Q99" s="3">
+        <f>(Q100+Q98)/2</f>
+        <v>1.35765</v>
       </c>
       <c r="R99">
         <v>1.3814</v>
@@ -6489,6 +6681,10 @@
       <c r="A106">
         <v>18</v>
       </c>
+      <c r="B106" s="3">
+        <f>(B107+B105)/2</f>
+        <v>0.168935</v>
+      </c>
       <c r="C106">
         <v>0.12753</v>
       </c>
@@ -6518,6 +6714,10 @@
       </c>
       <c r="M106">
         <v>18</v>
+      </c>
+      <c r="N106" s="3">
+        <f>(N107+N105)/2</f>
+        <v>1.1131500000000001</v>
       </c>
       <c r="O106">
         <v>1.2345999999999999</v>
@@ -6693,6 +6893,10 @@
       <c r="C109">
         <v>0.21102000000000001</v>
       </c>
+      <c r="D109" s="3">
+        <f>(D110+D108)/2</f>
+        <v>0.227605</v>
+      </c>
       <c r="E109">
         <v>0.19954</v>
       </c>
@@ -6722,6 +6926,10 @@
       </c>
       <c r="O109">
         <v>0.68430000000000002</v>
+      </c>
+      <c r="P109" s="3">
+        <f>(P110+P108)/2</f>
+        <v>0.85945000000000005</v>
       </c>
       <c r="Q109">
         <v>0.70399999999999996</v>
@@ -7027,6 +7235,10 @@
       <c r="C114">
         <v>0.33445000000000003</v>
       </c>
+      <c r="D114" s="3">
+        <f>(D115+D113)/2</f>
+        <v>0.27759</v>
+      </c>
       <c r="E114">
         <v>0.27694000000000002</v>
       </c>
@@ -7056,6 +7268,10 @@
       </c>
       <c r="O114">
         <v>1.1769000000000001</v>
+      </c>
+      <c r="P114" s="3">
+        <f>(P115+P113)/2</f>
+        <v>0.73344999999999994</v>
       </c>
       <c r="Q114">
         <v>0.73350000000000004</v>
@@ -7160,6 +7376,10 @@
       <c r="D116">
         <v>0.30492000000000002</v>
       </c>
+      <c r="E116" s="3">
+        <f>(E117+E115)/2</f>
+        <v>0.30308000000000002</v>
+      </c>
       <c r="F116">
         <v>0.35185</v>
       </c>
@@ -7169,6 +7389,10 @@
       <c r="H116">
         <v>0.30047000000000001</v>
       </c>
+      <c r="I116" s="3">
+        <f>(I117+I115)/2</f>
+        <v>0.325235</v>
+      </c>
       <c r="J116">
         <v>0.29361999999999999</v>
       </c>
@@ -7187,6 +7411,10 @@
       <c r="P116">
         <v>0.75219999999999998</v>
       </c>
+      <c r="Q116" s="3">
+        <f>(Q117+Q115)/2</f>
+        <v>0.75530000000000008</v>
+      </c>
       <c r="R116">
         <v>1.2347999999999999</v>
       </c>
@@ -7195,6 +7423,10 @@
       </c>
       <c r="T116">
         <v>0.7571</v>
+      </c>
+      <c r="U116" s="3">
+        <f>(U117+U115)/2</f>
+        <v>1.27</v>
       </c>
       <c r="V116">
         <v>1.3101</v>
@@ -7416,6 +7648,10 @@
       <c r="D122">
         <v>0.30731000000000003</v>
       </c>
+      <c r="E122" s="3">
+        <f>(E123+E121)/2</f>
+        <v>125000.146975</v>
+      </c>
       <c r="G122">
         <v>0.23877000000000001</v>
       </c>
@@ -7466,6 +7702,10 @@
       <c r="B123">
         <v>0.30064999999999997</v>
       </c>
+      <c r="C123" s="3">
+        <f>(C124+C122)/2</f>
+        <v>0.29814499999999999</v>
+      </c>
       <c r="D123">
         <v>0.29516999999999999</v>
       </c>
@@ -7492,6 +7732,10 @@
       </c>
       <c r="N123">
         <v>-0.74829999999999997</v>
+      </c>
+      <c r="O123" s="3">
+        <f>(O124+O122)/2</f>
+        <v>-0.74785000000000001</v>
       </c>
       <c r="P123">
         <v>-0.74819999999999998</v>
@@ -7744,6 +7988,10 @@
       <c r="J127">
         <v>0.23599999999999999</v>
       </c>
+      <c r="K127" s="3">
+        <f>(K128+K126)/2</f>
+        <v>0.23065999999999998</v>
+      </c>
       <c r="M127">
         <v>-20</v>
       </c>
@@ -7773,6 +8021,10 @@
       </c>
       <c r="V127">
         <v>-0.61880000000000002</v>
+      </c>
+      <c r="W127" s="3">
+        <f>(W128+W126)/2</f>
+        <v>-0.62909999999999999</v>
       </c>
     </row>
     <row r="128" spans="1:23">
@@ -7868,6 +8120,10 @@
       <c r="I129">
         <v>0.16034000000000001</v>
       </c>
+      <c r="K129" s="3">
+        <f>(K130+K128)/2</f>
+        <v>0.186915</v>
+      </c>
       <c r="M129">
         <v>-18</v>
       </c>
@@ -7891,6 +8147,10 @@
       </c>
       <c r="U129">
         <v>-0.30680000000000002</v>
+      </c>
+      <c r="W129" s="3">
+        <f>(W130+W128)/2</f>
+        <v>-0.61604999999999999</v>
       </c>
     </row>
     <row r="130" spans="1:23">
@@ -7971,6 +8231,10 @@
       <c r="G131">
         <v>0.14477999999999999</v>
       </c>
+      <c r="I131" s="3">
+        <f>(I132+I130)/2</f>
+        <v>0.11393</v>
+      </c>
       <c r="J131">
         <v>0.11543</v>
       </c>
@@ -7997,6 +8261,10 @@
       </c>
       <c r="S131">
         <v>-0.26090000000000002</v>
+      </c>
+      <c r="U131" s="3">
+        <f>(U132+U130)/2</f>
+        <v>-0.83529999999999993</v>
       </c>
       <c r="V131">
         <v>-0.76319999999999999</v>
@@ -8707,6 +8975,10 @@
       <c r="G142">
         <v>1.1610000000000001E-2</v>
       </c>
+      <c r="H142" s="3">
+        <f>(H143+H141)/2</f>
+        <v>1.1894999999999999E-2</v>
+      </c>
       <c r="I142">
         <v>8.2799999999999992E-3</v>
       </c>
@@ -8736,6 +9008,10 @@
       </c>
       <c r="S142">
         <v>-0.15129999999999999</v>
+      </c>
+      <c r="T142" s="3">
+        <f>(T143+T141)/2</f>
+        <v>-0.15195</v>
       </c>
       <c r="U142">
         <v>-0.1666</v>
@@ -8899,6 +9175,10 @@
       <c r="E145">
         <v>1.1639999999999999E-2</v>
       </c>
+      <c r="F145" s="3">
+        <f>(F146+F144)/2</f>
+        <v>9.2350000000000002E-3</v>
+      </c>
       <c r="G145">
         <v>8.4700000000000001E-3</v>
       </c>
@@ -8928,6 +9208,10 @@
       </c>
       <c r="Q145">
         <v>0.1837</v>
+      </c>
+      <c r="R145" s="3">
+        <f>(R146+R144)/2</f>
+        <v>0.18109999999999998</v>
       </c>
       <c r="S145">
         <v>0.1802</v>
@@ -9029,6 +9313,10 @@
       <c r="E147">
         <v>9.0200000000000002E-3</v>
       </c>
+      <c r="F147" s="3">
+        <f>(F148+F146)/2</f>
+        <v>7.5799999999999999E-3</v>
+      </c>
       <c r="G147">
         <v>6.9100000000000003E-3</v>
       </c>
@@ -9058,6 +9346,10 @@
       </c>
       <c r="Q147">
         <v>0.45290000000000002</v>
+      </c>
+      <c r="R147" s="3">
+        <f>(R148+R146)/2</f>
+        <v>0.42059999999999997</v>
       </c>
       <c r="S147">
         <v>0.39950000000000002</v>
@@ -9718,6 +10010,10 @@
       <c r="J157">
         <v>1.4579999999999999E-2</v>
       </c>
+      <c r="K157" s="3">
+        <f>(K158+K156)/2</f>
+        <v>1.3785E-2</v>
+      </c>
       <c r="M157">
         <v>10</v>
       </c>
@@ -9747,6 +10043,10 @@
       </c>
       <c r="V157">
         <v>1.431</v>
+      </c>
+      <c r="W157" s="3">
+        <f>(W158+W156)/2</f>
+        <v>1.4412499999999999</v>
       </c>
     </row>
     <row r="158" spans="1:23">
@@ -10634,6 +10934,10 @@
       <c r="G171">
         <v>0.24790999999999999</v>
       </c>
+      <c r="H171" s="3">
+        <f>(H172+H170)/2</f>
+        <v>0.28259000000000001</v>
+      </c>
       <c r="I171">
         <v>0.24396000000000001</v>
       </c>
@@ -10660,6 +10964,10 @@
       </c>
       <c r="S171">
         <v>0.72540000000000004</v>
+      </c>
+      <c r="T171" s="3">
+        <f>(T172+T170)/2</f>
+        <v>1.1758999999999999</v>
       </c>
       <c r="U171">
         <v>1.2545999999999999</v>
@@ -10755,6 +11063,10 @@
       <c r="H173">
         <v>0.33765000000000001</v>
       </c>
+      <c r="I173" s="3">
+        <f>(I174+I172)/2</f>
+        <v>0.27654000000000001</v>
+      </c>
       <c r="J173">
         <v>0.27728999999999998</v>
       </c>
@@ -10781,6 +11093,10 @@
       </c>
       <c r="T173">
         <v>1.1957</v>
+      </c>
+      <c r="U173" s="3">
+        <f>(U174+U172)/2</f>
+        <v>1.0060500000000001</v>
       </c>
       <c r="V173">
         <v>1.2796000000000001</v>
@@ -10929,6 +11245,10 @@
       <c r="J176">
         <v>0.37034</v>
       </c>
+      <c r="K176" s="3">
+        <f>(K177+K175)/2</f>
+        <v>0.34299999999999997</v>
+      </c>
       <c r="M176">
         <v>29</v>
       </c>
@@ -10955,6 +11275,10 @@
       </c>
       <c r="V176">
         <v>1.2824</v>
+      </c>
+      <c r="W176" s="3">
+        <f>(W177+W175)/2</f>
+        <v>1.30935</v>
       </c>
     </row>
     <row r="177" spans="1:23">
@@ -11152,6 +11476,10 @@
       <c r="B182">
         <v>0.30823</v>
       </c>
+      <c r="C182" s="3">
+        <f>(C183+C181)/2</f>
+        <v>0.30456</v>
+      </c>
       <c r="D182">
         <v>0.23530000000000001</v>
       </c>
@@ -11172,6 +11500,10 @@
       </c>
       <c r="N182">
         <v>-0.76400000000000001</v>
+      </c>
+      <c r="O182" s="3">
+        <f>(O183+O181)/2</f>
+        <v>-0.76285000000000003</v>
       </c>
       <c r="P182">
         <v>-0.43690000000000001</v>
@@ -11214,6 +11546,10 @@
       <c r="J183">
         <v>0.28100999999999998</v>
       </c>
+      <c r="K183" s="3">
+        <f>(K184+K182)/2</f>
+        <v>0.24415500000000001</v>
+      </c>
       <c r="M183">
         <v>-23</v>
       </c>
@@ -11237,6 +11573,10 @@
       </c>
       <c r="V183">
         <v>-0.73380000000000001</v>
+      </c>
+      <c r="W183" s="3">
+        <f>(W184+W182)/2</f>
+        <v>-0.57274999999999998</v>
       </c>
     </row>
     <row r="184" spans="1:23">
@@ -11355,6 +11695,10 @@
       <c r="A186">
         <v>-20</v>
       </c>
+      <c r="B186" s="3">
+        <f>(B187+B185)/2</f>
+        <v>0.24885499999999999</v>
+      </c>
       <c r="C186">
         <v>0.25502000000000002</v>
       </c>
@@ -11367,6 +11711,10 @@
       <c r="H186">
         <v>0.24346999999999999</v>
       </c>
+      <c r="I186" s="3">
+        <f>(I187+I185)/2</f>
+        <v>0.21195</v>
+      </c>
       <c r="J186">
         <v>0.24088999999999999</v>
       </c>
@@ -11376,6 +11724,10 @@
       <c r="M186">
         <v>-20</v>
       </c>
+      <c r="N186" s="3">
+        <f>(N187+N185)/2</f>
+        <v>-0.61194999999999999</v>
+      </c>
       <c r="O186">
         <v>-0.61919999999999997</v>
       </c>
@@ -11387,6 +11739,10 @@
       </c>
       <c r="T186">
         <v>-0.61699999999999999</v>
+      </c>
+      <c r="U186" s="3">
+        <f>(U187+U185)/2</f>
+        <v>-0.47745000000000004</v>
       </c>
       <c r="V186">
         <v>-0.62370000000000003</v>
@@ -11762,6 +12118,10 @@
       <c r="H193">
         <v>0.14137</v>
       </c>
+      <c r="I193" s="3">
+        <f>(I194+I192)/2</f>
+        <v>9.3075000000000005E-2</v>
+      </c>
       <c r="J193">
         <v>3.2239999999999998E-2</v>
       </c>
@@ -11791,6 +12151,10 @@
       </c>
       <c r="T193">
         <v>-0.40550000000000003</v>
+      </c>
+      <c r="U193" s="3">
+        <f>(U194+U192)/2</f>
+        <v>-0.66690000000000005</v>
       </c>
       <c r="V193">
         <v>-1.0467</v>
@@ -11892,6 +12256,10 @@
       <c r="H195">
         <v>0.10672</v>
       </c>
+      <c r="I195" s="3">
+        <f>(I196+I194)/2</f>
+        <v>3.3485000000000001E-2</v>
+      </c>
       <c r="J195">
         <v>1.703E-2</v>
       </c>
@@ -11921,6 +12289,10 @@
       </c>
       <c r="T195">
         <v>-0.38950000000000001</v>
+      </c>
+      <c r="U195" s="3">
+        <f>(U196+U194)/2</f>
+        <v>-0.7752</v>
       </c>
       <c r="V195">
         <v>-0.87719999999999998</v>
@@ -12140,12 +12512,20 @@
       <c r="B199">
         <v>8.9380000000000001E-2</v>
       </c>
+      <c r="C199" s="3">
+        <f>(C200+C198)/2</f>
+        <v>8.0464999999999995E-2</v>
+      </c>
       <c r="D199">
         <v>7.6749999999999999E-2</v>
       </c>
       <c r="E199">
         <v>6.615E-2</v>
       </c>
+      <c r="F199" s="3">
+        <f>(F200+F198)/2</f>
+        <v>4.5574999999999997E-2</v>
+      </c>
       <c r="G199">
         <v>2.1850000000000001E-2</v>
       </c>
@@ -12167,11 +12547,19 @@
       <c r="N199">
         <v>-0.39069999999999999</v>
       </c>
+      <c r="O199" s="3">
+        <f>(O200+O198)/2</f>
+        <v>-0.38590000000000002</v>
+      </c>
       <c r="P199">
         <v>-0.37340000000000001</v>
       </c>
       <c r="Q199">
         <v>-0.32769999999999999</v>
+      </c>
+      <c r="R199" s="3">
+        <f>(R200+R198)/2</f>
+        <v>-0.29610000000000003</v>
       </c>
       <c r="S199">
         <v>-0.35949999999999999</v>
@@ -12211,6 +12599,10 @@
       <c r="G200">
         <v>1.6109999999999999E-2</v>
       </c>
+      <c r="H200" s="3">
+        <f>(H201+H199)/2</f>
+        <v>1.6590000000000001E-2</v>
+      </c>
       <c r="I200">
         <v>1.072E-2</v>
       </c>
@@ -12240,6 +12632,10 @@
       </c>
       <c r="S200">
         <v>-0.26479999999999998</v>
+      </c>
+      <c r="T200" s="3">
+        <f>(T201+T199)/2</f>
+        <v>-0.26114999999999999</v>
       </c>
       <c r="U200">
         <v>-0.28639999999999999</v>
@@ -12542,6 +12938,10 @@
       <c r="F205">
         <v>8.4799999999999997E-3</v>
       </c>
+      <c r="G205" s="3">
+        <f>(G206+G204)/2</f>
+        <v>7.8849999999999996E-3</v>
+      </c>
       <c r="H205">
         <v>7.6299999999999996E-3</v>
       </c>
@@ -12571,6 +12971,10 @@
       </c>
       <c r="R205">
         <v>0.2989</v>
+      </c>
+      <c r="S205" s="3">
+        <f>(S206+S204)/2</f>
+        <v>0.29820000000000002</v>
       </c>
       <c r="T205">
         <v>0.30020000000000002</v>
@@ -12616,6 +13020,10 @@
       <c r="J206">
         <v>6.3800000000000003E-3</v>
       </c>
+      <c r="K206" s="3">
+        <f>(K207+K205)/2</f>
+        <v>6.2400000000000008E-3</v>
+      </c>
       <c r="M206">
         <v>0</v>
       </c>
@@ -12645,6 +13053,10 @@
       </c>
       <c r="V206">
         <v>0.41749999999999998</v>
+      </c>
+      <c r="W206" s="3">
+        <f>(W207+W205)/2</f>
+        <v>0.41559999999999997</v>
       </c>
     </row>
     <row r="207" spans="1:23">
@@ -13263,6 +13675,10 @@
       <c r="A216">
         <v>10</v>
       </c>
+      <c r="B216" s="3">
+        <f>(B217+B215)/2</f>
+        <v>3.3225000000000005E-2</v>
+      </c>
       <c r="C216">
         <v>2.7550000000000002E-2</v>
       </c>
@@ -13292,6 +13708,10 @@
       </c>
       <c r="M216">
         <v>10</v>
+      </c>
+      <c r="N216" s="3">
+        <f>(N217+N215)/2</f>
+        <v>1.3211499999999998</v>
       </c>
       <c r="O216">
         <v>1.3154999999999999</v>
@@ -13535,6 +13955,10 @@
       <c r="C220">
         <v>7.6240000000000002E-2</v>
       </c>
+      <c r="D220" s="3">
+        <f>(D221+D219)/2</f>
+        <v>7.4045E-2</v>
+      </c>
       <c r="E220">
         <v>7.1040000000000006E-2</v>
       </c>
@@ -13564,6 +13988,10 @@
       </c>
       <c r="O220">
         <v>1.2736000000000001</v>
+      </c>
+      <c r="P220" s="3">
+        <f>(P221+P219)/2</f>
+        <v>1.29955</v>
       </c>
       <c r="Q220">
         <v>1.3179000000000001</v>
@@ -14224,6 +14652,10 @@
       <c r="H230">
         <v>0.25013999999999997</v>
       </c>
+      <c r="I230" s="3">
+        <f>(I231+I229)/2</f>
+        <v>0.262465</v>
+      </c>
       <c r="J230">
         <v>0.27071000000000001</v>
       </c>
@@ -14253,6 +14685,10 @@
       </c>
       <c r="T230">
         <v>0.74099999999999999</v>
+      </c>
+      <c r="U230" s="3">
+        <f>(U231+U229)/2</f>
+        <v>0.97384999999999999</v>
       </c>
       <c r="V230">
         <v>1.2316</v>
@@ -14357,6 +14793,10 @@
       <c r="I232">
         <v>0.28136</v>
       </c>
+      <c r="K232" s="3">
+        <f>(K233+K231)/2</f>
+        <v>0.32144499999999998</v>
+      </c>
       <c r="M232">
         <v>26</v>
       </c>
@@ -14383,6 +14823,10 @@
       </c>
       <c r="U232">
         <v>0.76029999999999998</v>
+      </c>
+      <c r="W232" s="3">
+        <f>(W233+W231)/2</f>
+        <v>1.25665</v>
       </c>
     </row>
     <row r="233" spans="1:23">
@@ -14546,6 +14990,10 @@
       <c r="J235">
         <v>0.32361000000000001</v>
       </c>
+      <c r="K235" s="3">
+        <f>(K236+K234)/2</f>
+        <v>0.35278500000000002</v>
+      </c>
       <c r="M235">
         <v>29</v>
       </c>
@@ -14575,6 +15023,10 @@
       </c>
       <c r="V235">
         <v>0.79259999999999997</v>
+      </c>
+      <c r="W235" s="3">
+        <f>(W236+W234)/2</f>
+        <v>1.04545</v>
       </c>
     </row>
     <row r="236" spans="1:23">
@@ -14781,6 +15233,10 @@
       <c r="A241">
         <v>-24</v>
       </c>
+      <c r="B241" s="3">
+        <f>(B242+B240)/2</f>
+        <v>0.31133500000000003</v>
+      </c>
       <c r="C241">
         <v>0.31224000000000002</v>
       </c>
@@ -14804,6 +15260,10 @@
       </c>
       <c r="M241">
         <v>-24</v>
+      </c>
+      <c r="N241" s="3">
+        <f>(N242+N240)/2</f>
+        <v>-0.78620000000000001</v>
       </c>
       <c r="O241">
         <v>-0.78749999999999998</v>
@@ -14961,6 +15421,10 @@
       <c r="H244">
         <v>0.19836999999999999</v>
       </c>
+      <c r="I244" s="3">
+        <f>(I245+I243)/2</f>
+        <v>0.19821</v>
+      </c>
       <c r="J244">
         <v>0.26172000000000001</v>
       </c>
@@ -14987,6 +15451,10 @@
       </c>
       <c r="T244">
         <v>-0.37730000000000002</v>
+      </c>
+      <c r="U244" s="3">
+        <f>(U245+U243)/2</f>
+        <v>-0.3755</v>
       </c>
       <c r="V244">
         <v>-0.67449999999999999</v>
@@ -15880,6 +16348,10 @@
       <c r="D258">
         <v>8.0869999999999997E-2</v>
       </c>
+      <c r="E258" s="3">
+        <f>(E259+E257)/2</f>
+        <v>7.233500000000001E-2</v>
+      </c>
       <c r="F258">
         <v>3.8899999999999997E-2</v>
       </c>
@@ -15909,6 +16381,10 @@
       </c>
       <c r="P258">
         <v>-0.33019999999999999</v>
+      </c>
+      <c r="Q258" s="3">
+        <f>(Q259+Q257)/2</f>
+        <v>-0.28565000000000002</v>
       </c>
       <c r="R258">
         <v>-0.29980000000000001</v>
@@ -15945,6 +16421,10 @@
       <c r="E259">
         <v>5.2330000000000002E-2</v>
       </c>
+      <c r="F259" s="3">
+        <f>(F260+F258)/2</f>
+        <v>2.8199999999999999E-2</v>
+      </c>
       <c r="G259">
         <v>2.0760000000000001E-2</v>
       </c>
@@ -15974,6 +16454,10 @@
       </c>
       <c r="Q259">
         <v>-0.22459999999999999</v>
+      </c>
+      <c r="R259" s="3">
+        <f>(R260+R258)/2</f>
+        <v>-0.22665000000000002</v>
       </c>
       <c r="S259">
         <v>-0.26590000000000003</v>
@@ -16489,6 +16973,10 @@
       <c r="G267">
         <v>6.9199999999999999E-3</v>
       </c>
+      <c r="H267" s="3">
+        <f>(H268+H266)/2</f>
+        <v>6.9300000000000004E-3</v>
+      </c>
       <c r="I267">
         <v>6.1199999999999996E-3</v>
       </c>
@@ -16518,6 +17006,10 @@
       </c>
       <c r="S267">
         <v>0.70279999999999998</v>
+      </c>
+      <c r="T267" s="3">
+        <f>(T268+T266)/2</f>
+        <v>0.67259999999999998</v>
       </c>
       <c r="U267">
         <v>0.6603</v>
@@ -16613,6 +17105,10 @@
       <c r="E269">
         <v>1.2E-2</v>
       </c>
+      <c r="F269" s="3">
+        <f>(F270+F268)/2</f>
+        <v>9.8549999999999992E-3</v>
+      </c>
       <c r="G269">
         <v>9.0500000000000008E-3</v>
       </c>
@@ -16642,6 +17138,10 @@
       </c>
       <c r="Q269">
         <v>0.89410000000000001</v>
+      </c>
+      <c r="R269" s="3">
+        <f>(R270+R268)/2</f>
+        <v>0.89765000000000006</v>
       </c>
       <c r="S269">
         <v>0.89910000000000001</v>
@@ -17148,6 +17648,10 @@
       <c r="D277">
         <v>5.1409999999999997E-2</v>
       </c>
+      <c r="E277" s="3">
+        <f>(E278+E276)/2</f>
+        <v>5.2859999999999997E-2</v>
+      </c>
       <c r="F277">
         <v>4.6080000000000003E-2</v>
       </c>
@@ -17177,6 +17681,10 @@
       </c>
       <c r="P277">
         <v>1.3387</v>
+      </c>
+      <c r="Q277" s="3">
+        <f>(Q278+Q276)/2</f>
+        <v>1.3367499999999999</v>
       </c>
       <c r="R277">
         <v>1.393</v>
@@ -17683,6 +18191,10 @@
       <c r="C285">
         <v>0.26904</v>
       </c>
+      <c r="D285" s="3">
+        <f>(D286+D284)/2</f>
+        <v>0.25962499999999999</v>
+      </c>
       <c r="E285">
         <v>0.25992999999999999</v>
       </c>
@@ -17712,6 +18224,10 @@
       </c>
       <c r="O285">
         <v>1.0758000000000001</v>
+      </c>
+      <c r="P285" s="3">
+        <f>(P286+P284)/2</f>
+        <v>1.07125</v>
       </c>
       <c r="Q285">
         <v>1.0680000000000001</v>
@@ -17943,6 +18459,10 @@
       <c r="A289">
         <v>24</v>
       </c>
+      <c r="B289" s="3">
+        <f>(B290+B288)/2</f>
+        <v>0.33523000000000003</v>
+      </c>
       <c r="C289">
         <v>0.33387</v>
       </c>
@@ -17972,6 +18492,10 @@
       </c>
       <c r="M289">
         <v>24</v>
+      </c>
+      <c r="N289" s="3">
+        <f>(N290+N288)/2</f>
+        <v>1.1991499999999999</v>
       </c>
       <c r="O289">
         <v>1.2011000000000001</v>
@@ -18032,6 +18556,10 @@
       <c r="J290">
         <v>0.34706999999999999</v>
       </c>
+      <c r="K290" s="3">
+        <f>(K291+K289)/2</f>
+        <v>0.34210499999999999</v>
+      </c>
       <c r="M290">
         <v>25</v>
       </c>
@@ -18061,6 +18589,10 @@
       </c>
       <c r="V290">
         <v>1.2382</v>
+      </c>
+      <c r="W290" s="3">
+        <f>(W291+W289)/2</f>
+        <v>1.2410000000000001</v>
       </c>
     </row>
     <row r="291" spans="1:23">
@@ -18230,6 +18762,10 @@
       <c r="J293">
         <v>0.38796999999999998</v>
       </c>
+      <c r="K293" s="3">
+        <f>(K294+K292)/2</f>
+        <v>0.38677499999999998</v>
+      </c>
       <c r="M293">
         <v>28</v>
       </c>
@@ -18259,6 +18795,10 @@
       </c>
       <c r="V293">
         <v>1.3435999999999999</v>
+      </c>
+      <c r="W293" s="3">
+        <f>(W294+W292)/2</f>
+        <v>1.34195</v>
       </c>
     </row>
     <row r="294" spans="1:23">
@@ -18684,6 +19224,10 @@
       <c r="H302" s="1">
         <v>0.29481000000000002</v>
       </c>
+      <c r="I302" s="3">
+        <f>(I303+I301)/2</f>
+        <v>0.25266</v>
+      </c>
       <c r="K302">
         <v>0.28886000000000001</v>
       </c>
@@ -18710,6 +19254,10 @@
       </c>
       <c r="T302">
         <v>-0.7399</v>
+      </c>
+      <c r="U302" s="3">
+        <f>(U303+U301)/2</f>
+        <v>-0.56664999999999999</v>
       </c>
       <c r="W302">
         <v>-0.74409999999999998</v>
@@ -18719,6 +19267,14 @@
       <c r="A303">
         <v>-21</v>
       </c>
+      <c r="B303" s="3">
+        <f>(B304+B302)/2</f>
+        <v>0.28054999999999997</v>
+      </c>
+      <c r="C303" s="3">
+        <f>(C304+C302)/2</f>
+        <v>0.21244499999999999</v>
+      </c>
       <c r="D303" s="1">
         <v>0.27882000000000001</v>
       </c>
@@ -18742,6 +19298,14 @@
       </c>
       <c r="M303">
         <v>-21</v>
+      </c>
+      <c r="N303" s="3">
+        <f>(N304+N302)/2</f>
+        <v>-0.69199999999999995</v>
+      </c>
+      <c r="O303" s="3">
+        <f>(O304+O302)/2</f>
+        <v>-0.38724999999999998</v>
       </c>
       <c r="P303" s="1">
         <v>-0.69210000000000005</v>
@@ -18790,6 +19354,10 @@
       <c r="H304" s="1">
         <v>0.26022000000000001</v>
       </c>
+      <c r="I304" s="3">
+        <f>(I305+I303)/2</f>
+        <v>0.26026499999999997</v>
+      </c>
       <c r="K304">
         <v>0.25761000000000001</v>
       </c>
@@ -18816,6 +19384,10 @@
       </c>
       <c r="T304">
         <v>-0.64939999999999998</v>
+      </c>
+      <c r="U304" s="3">
+        <f>(U305+U303)/2</f>
+        <v>-0.65195000000000003</v>
       </c>
       <c r="W304">
         <v>-0.65529999999999999</v>
@@ -18887,6 +19459,10 @@
       <c r="A306">
         <v>-18</v>
       </c>
+      <c r="B306" s="3">
+        <f>(B307+B305)/2</f>
+        <v>0.23607999999999998</v>
+      </c>
       <c r="C306" s="1">
         <v>0.17888999999999999</v>
       </c>
@@ -18913,6 +19489,10 @@
       </c>
       <c r="M306">
         <v>-18</v>
+      </c>
+      <c r="N306" s="3">
+        <f>(N307+N305)/2</f>
+        <v>-0.55984999999999996</v>
       </c>
       <c r="O306" s="1">
         <v>-0.31369999999999998</v>
@@ -19463,6 +20043,10 @@
       <c r="I315" s="1">
         <v>0.08</v>
       </c>
+      <c r="K315" s="3">
+        <f>(K316+K314)/2</f>
+        <v>7.3120000000000004E-2</v>
+      </c>
       <c r="M315">
         <v>-9</v>
       </c>
@@ -19489,6 +20073,10 @@
       </c>
       <c r="U315">
         <v>-0.30790000000000001</v>
+      </c>
+      <c r="W315" s="3">
+        <f>(W316+W314)/2</f>
+        <v>-0.36845</v>
       </c>
     </row>
     <row r="316" spans="1:23">
@@ -19578,6 +20166,10 @@
       <c r="H317" s="1">
         <v>5.3240000000000003E-2</v>
       </c>
+      <c r="I317" s="3">
+        <f>(I318+I316)/2</f>
+        <v>4.1215000000000002E-2</v>
+      </c>
       <c r="J317" s="1">
         <v>2.7E-2</v>
       </c>
@@ -19607,6 +20199,10 @@
       </c>
       <c r="T317">
         <v>-0.26129999999999998</v>
+      </c>
+      <c r="U317" s="3">
+        <f>(U318+U316)/2</f>
+        <v>-0.30869999999999997</v>
       </c>
       <c r="V317">
         <v>-0.39150000000000001</v>
@@ -20033,6 +20629,10 @@
       <c r="C324" s="1">
         <v>1.374E-2</v>
       </c>
+      <c r="D324" s="3">
+        <f>(D325+D323)/2</f>
+        <v>1.2215E-2</v>
+      </c>
       <c r="E324" s="1">
         <v>9.9100000000000004E-3</v>
       </c>
@@ -20062,6 +20662,10 @@
       </c>
       <c r="O324" s="1">
         <v>0.49299999999999999</v>
+      </c>
+      <c r="P324" s="3">
+        <f>(P325+P323)/2</f>
+        <v>0.46984999999999999</v>
       </c>
       <c r="Q324" s="1">
         <v>0.43659999999999999</v>
@@ -20586,6 +21190,10 @@
       <c r="H332" s="1">
         <v>1.7180000000000001E-2</v>
       </c>
+      <c r="I332" s="3">
+        <f>(I333+I331)/2</f>
+        <v>1.6070000000000001E-2</v>
+      </c>
       <c r="J332" s="1">
         <v>1.482E-2</v>
       </c>
@@ -20615,6 +21223,10 @@
       </c>
       <c r="T332">
         <v>1.3391</v>
+      </c>
+      <c r="U332" s="3">
+        <f>(U333+U331)/2</f>
+        <v>1.3635000000000002</v>
       </c>
       <c r="V332">
         <v>1.3801000000000001</v>
@@ -20908,6 +21520,10 @@
       <c r="D337" s="1">
         <v>9.2119999999999994E-2</v>
       </c>
+      <c r="E337" s="3">
+        <f>(E338+E336)/2</f>
+        <v>9.0560000000000002E-2</v>
+      </c>
       <c r="F337" s="1">
         <v>8.5669999999999996E-2</v>
       </c>
@@ -20937,6 +21553,10 @@
       </c>
       <c r="P337" s="1">
         <v>1.2276</v>
+      </c>
+      <c r="Q337" s="3">
+        <f>(Q338+Q336)/2</f>
+        <v>1.2524999999999999</v>
       </c>
       <c r="R337" s="1">
         <v>1.2966</v>
@@ -21301,6 +21921,10 @@
       <c r="A343">
         <v>19</v>
       </c>
+      <c r="B343" s="3">
+        <f>(B344+B342)/2</f>
+        <v>0.26417499999999999</v>
+      </c>
       <c r="C343" s="1">
         <v>0.25756000000000001</v>
       </c>
@@ -21330,6 +21954,10 @@
       </c>
       <c r="M343">
         <v>19</v>
+      </c>
+      <c r="N343" s="3">
+        <f>(N344+N342)/2</f>
+        <v>1.0686</v>
       </c>
       <c r="O343" s="1">
         <v>1.0757000000000001</v>
@@ -21375,6 +22003,10 @@
       <c r="E344" s="1">
         <v>0.27681</v>
       </c>
+      <c r="F344" s="3">
+        <f>(F345+F343)/2</f>
+        <v>0.26927000000000001</v>
+      </c>
       <c r="G344" s="1">
         <v>0.26590999999999998</v>
       </c>
@@ -21404,6 +22036,10 @@
       </c>
       <c r="Q344" s="1">
         <v>1.1126</v>
+      </c>
+      <c r="R344" s="3">
+        <f>(R345+R343)/2</f>
+        <v>1.1245500000000002</v>
       </c>
       <c r="S344" s="1">
         <v>1.1276999999999999</v>
@@ -21833,6 +22469,10 @@
       <c r="A351">
         <v>27</v>
       </c>
+      <c r="B351" s="3">
+        <f>(B352+B350)/2</f>
+        <v>0.40725</v>
+      </c>
       <c r="C351" s="1">
         <v>0.40627999999999997</v>
       </c>
@@ -21862,6 +22502,10 @@
       </c>
       <c r="M351">
         <v>27</v>
+      </c>
+      <c r="N351" s="3">
+        <f>(N352+N350)/2</f>
+        <v>1.3891</v>
       </c>
       <c r="O351" s="1">
         <v>1.3903000000000001</v>
@@ -22293,6 +22937,10 @@
       <c r="C360" s="1">
         <v>0.33761999999999998</v>
       </c>
+      <c r="D360" s="3">
+        <f>(D361+D359)/2</f>
+        <v>0.34023999999999999</v>
+      </c>
       <c r="E360" s="1">
         <v>0.33778999999999998</v>
       </c>
@@ -22319,6 +22967,10 @@
       </c>
       <c r="O360">
         <v>-0.84099999999999997</v>
+      </c>
+      <c r="P360" s="3">
+        <f>(P361+P359)/2</f>
+        <v>-0.84034999999999993</v>
       </c>
       <c r="Q360">
         <v>-0.84050000000000002</v>
@@ -22343,6 +22995,10 @@
       <c r="A361">
         <v>-22</v>
       </c>
+      <c r="B361" s="3">
+        <f>(B362+B360)/2</f>
+        <v>0.31986500000000001</v>
+      </c>
       <c r="C361" s="1">
         <v>0.32296999999999998</v>
       </c>
@@ -22369,6 +23025,10 @@
       </c>
       <c r="M361">
         <v>-22</v>
+      </c>
+      <c r="N361" s="3">
+        <f>(N362+N360)/2</f>
+        <v>-0.7893</v>
       </c>
       <c r="O361" s="1">
         <v>-0.78910000000000002</v>
@@ -22402,6 +23062,10 @@
       <c r="B362" s="1">
         <v>0.30125000000000002</v>
       </c>
+      <c r="C362" s="3">
+        <f>(C363+C361)/2</f>
+        <v>0.30244499999999996</v>
+      </c>
       <c r="D362" s="1">
         <v>0.29976999999999998</v>
       </c>
@@ -22425,6 +23089,10 @@
       </c>
       <c r="N362" s="1">
         <v>-0.73750000000000004</v>
+      </c>
+      <c r="O362" s="4">
+        <f>(O363+O361)/2</f>
+        <v>-0.73694999999999999</v>
       </c>
       <c r="P362" s="1">
         <v>-0.73660000000000003</v>
@@ -22511,6 +23179,10 @@
       <c r="A364">
         <v>-19</v>
       </c>
+      <c r="B364" s="3">
+        <f>(B365+B363)/2</f>
+        <v>0.26602500000000001</v>
+      </c>
       <c r="C364" s="1">
         <v>0.26428000000000001</v>
       </c>
@@ -22537,6 +23209,10 @@
       </c>
       <c r="M364">
         <v>-19</v>
+      </c>
+      <c r="N364" s="3">
+        <f>(N365+N363)/2</f>
+        <v>-0.63424999999999998</v>
       </c>
       <c r="O364" s="1">
         <v>-0.63270000000000004</v>
@@ -22573,6 +23249,10 @@
       <c r="C365" s="1">
         <v>0.24939</v>
       </c>
+      <c r="D365" s="3">
+        <f>(D366+D364)/2</f>
+        <v>0.248365</v>
+      </c>
       <c r="E365" s="1">
         <v>0.24610000000000001</v>
       </c>
@@ -22599,6 +23279,10 @@
       </c>
       <c r="O365" s="1">
         <v>-0.58379999999999999</v>
+      </c>
+      <c r="P365" s="3">
+        <f>(P366+P364)/2</f>
+        <v>-0.58330000000000004</v>
       </c>
       <c r="Q365">
         <v>-0.58089999999999997</v>
@@ -22889,6 +23573,10 @@
       <c r="C370" s="1">
         <v>0.16663</v>
       </c>
+      <c r="D370" s="3">
+        <f>(D371+D369)/2</f>
+        <v>0.16813500000000001</v>
+      </c>
       <c r="E370" s="1">
         <v>0.16352</v>
       </c>
@@ -22918,6 +23606,10 @@
       </c>
       <c r="O370" s="1">
         <v>-0.35549999999999998</v>
+      </c>
+      <c r="P370" s="3">
+        <f>(P371+P369)/2</f>
+        <v>-0.36480000000000001</v>
       </c>
       <c r="Q370" s="1">
         <v>-0.35580000000000001</v>
@@ -22945,6 +23637,10 @@
       <c r="A371">
         <v>-12</v>
       </c>
+      <c r="B371" s="3">
+        <f>(B372+B370)/2</f>
+        <v>0.15569</v>
+      </c>
       <c r="C371" s="1">
         <v>0.1532</v>
       </c>
@@ -22974,6 +23670,10 @@
       </c>
       <c r="M371">
         <v>-12</v>
+      </c>
+      <c r="N371" s="3">
+        <f>(N372+N370)/2</f>
+        <v>-0.32445000000000002</v>
       </c>
       <c r="O371">
         <v>-0.32029999999999997</v>
@@ -23034,6 +23734,10 @@
       <c r="J372">
         <v>0.11916</v>
       </c>
+      <c r="K372" s="3">
+        <f>(K373+K371)/2</f>
+        <v>0.11816499999999999</v>
+      </c>
       <c r="M372">
         <v>-11</v>
       </c>
@@ -23063,6 +23767,10 @@
       </c>
       <c r="V372">
         <v>-0.31890000000000002</v>
+      </c>
+      <c r="W372" s="3">
+        <f>(W373+W371)/2</f>
+        <v>-0.32484999999999997</v>
       </c>
     </row>
     <row r="373" spans="1:23">
@@ -23545,6 +24253,10 @@
       <c r="A380">
         <v>-3</v>
       </c>
+      <c r="B380" s="3">
+        <f>(B381+B379)/2</f>
+        <v>4.4084999999999999E-2</v>
+      </c>
       <c r="C380" s="1">
         <v>2.7980000000000001E-2</v>
       </c>
@@ -23574,6 +24286,10 @@
       </c>
       <c r="M380">
         <v>-3</v>
+      </c>
+      <c r="N380" s="3">
+        <f>(N381+N379)/2</f>
+        <v>-0.1087</v>
       </c>
       <c r="O380" s="1">
         <v>3.3999999999999998E-3</v>
@@ -23699,6 +24415,10 @@
       <c r="I382" s="1">
         <v>7.5100000000000002E-3</v>
       </c>
+      <c r="J382" s="3">
+        <f>(J383+J381)/2</f>
+        <v>7.2899999999999996E-3</v>
+      </c>
       <c r="K382">
         <v>6.8199999999999997E-3</v>
       </c>
@@ -23728,6 +24448,10 @@
       </c>
       <c r="U382">
         <v>0.35899999999999999</v>
+      </c>
+      <c r="V382" s="3">
+        <f>(V383+V381)/2</f>
+        <v>0.35735</v>
       </c>
       <c r="W382">
         <v>0.36020000000000002</v>
@@ -23758,6 +24482,10 @@
       <c r="H383" s="1">
         <v>8.1300000000000001E-3</v>
       </c>
+      <c r="I383" s="3">
+        <f>(I384+I382)/2</f>
+        <v>7.6699999999999997E-3</v>
+      </c>
       <c r="J383">
         <v>7.3299999999999997E-3</v>
       </c>
@@ -23787,6 +24515,10 @@
       </c>
       <c r="T383">
         <v>0.49559999999999998</v>
+      </c>
+      <c r="U383" s="3">
+        <f>(U384+U382)/2</f>
+        <v>0.49404999999999999</v>
       </c>
       <c r="V383">
         <v>0.50080000000000002</v>
@@ -23811,6 +24543,10 @@
       <c r="E384" s="1">
         <v>1.0840000000000001E-2</v>
       </c>
+      <c r="F384" s="3">
+        <f>(F385+F383)/2</f>
+        <v>9.2300000000000004E-3</v>
+      </c>
       <c r="G384" s="1">
         <v>7.9000000000000008E-3</v>
       </c>
@@ -23840,6 +24576,10 @@
       </c>
       <c r="Q384" s="1">
         <v>0.66859999999999997</v>
+      </c>
+      <c r="R384" s="3">
+        <f>(R385+R383)/2</f>
+        <v>0.63430000000000009</v>
       </c>
       <c r="S384" s="1">
         <v>0.62090000000000001</v>
@@ -24083,6 +24823,10 @@
       <c r="G388" s="1">
         <v>1.225E-2</v>
       </c>
+      <c r="H388" s="3">
+        <f>(H389+H387)/2</f>
+        <v>1.149E-2</v>
+      </c>
       <c r="I388" s="1">
         <v>9.2300000000000004E-3</v>
       </c>
@@ -24112,6 +24856,10 @@
       </c>
       <c r="S388">
         <v>1.1154999999999999</v>
+      </c>
+      <c r="T388" s="3">
+        <f>(T389+T387)/2</f>
+        <v>1.1335999999999999</v>
       </c>
       <c r="U388">
         <v>1.1841999999999999</v>
@@ -24151,6 +24899,10 @@
       <c r="I389" s="1">
         <v>1.146E-2</v>
       </c>
+      <c r="J389" s="3">
+        <f>(J390+J388)/2</f>
+        <v>1.119E-2</v>
+      </c>
       <c r="K389">
         <v>1.082E-2</v>
       </c>
@@ -24180,6 +24932,10 @@
       </c>
       <c r="U389">
         <v>1.2823</v>
+      </c>
+      <c r="V389" s="3">
+        <f>(V390+V388)/2</f>
+        <v>1.2968999999999999</v>
       </c>
       <c r="W389">
         <v>1.2951999999999999</v>
@@ -25204,6 +25960,10 @@
       <c r="H407" s="1">
         <v>0.39288000000000001</v>
       </c>
+      <c r="J407" s="3">
+        <f>(J408+J406)/2</f>
+        <v>0.34819500000000003</v>
+      </c>
       <c r="M407">
         <v>24</v>
       </c>
@@ -25227,6 +25987,10 @@
       </c>
       <c r="T407">
         <v>1.3851</v>
+      </c>
+      <c r="V407" s="3">
+        <f>(V408+V406)/2</f>
+        <v>1.0935999999999999</v>
       </c>
     </row>
     <row r="408" spans="1:22">
@@ -25351,9 +26115,21 @@
       <c r="C410" s="1">
         <v>0.47119</v>
       </c>
+      <c r="D410" s="3">
+        <f>(D411+D409)/2</f>
+        <v>0.46516000000000002</v>
+      </c>
       <c r="E410" s="1">
         <v>0.46309</v>
       </c>
+      <c r="F410" s="3">
+        <f>(F411+F409)/2</f>
+        <v>0.41493500000000005</v>
+      </c>
+      <c r="G410" s="3">
+        <f>(G411+G409)/2</f>
+        <v>0.46018999999999999</v>
+      </c>
       <c r="H410" s="1">
         <v>0.45983000000000002</v>
       </c>
@@ -25369,8 +26145,20 @@
       <c r="O410" s="1">
         <v>1.5287999999999999</v>
       </c>
+      <c r="P410" s="3">
+        <f>(P411+P409)/2</f>
+        <v>1.5267499999999998</v>
+      </c>
       <c r="Q410" s="1">
         <v>1.5276000000000001</v>
+      </c>
+      <c r="R410" s="3">
+        <f>(R411+R409)/2</f>
+        <v>1.1858</v>
+      </c>
+      <c r="S410" s="3">
+        <f>(S411+S409)/2</f>
+        <v>1.5272000000000001</v>
       </c>
       <c r="T410">
         <v>1.5279</v>

</xml_diff>